<commit_message>
About to start binary search trees
</commit_message>
<xml_diff>
--- a/Exercise_Sequence.xlsx
+++ b/Exercise_Sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brind\Documents\HtDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F885FEF3-221B-4A77-BADC-7E164D1F5AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB8E7D-E963-46A6-B64C-AA17CDC6EDE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22016CAA-A539-451C-8737-08F3A468224D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="718">
   <si>
     <t>#</t>
   </si>
@@ -2185,6 +2185,9 @@
   </si>
   <si>
     <t>completed on 01.11.</t>
+  </si>
+  <si>
+    <t>completed on 07-Nov</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC50D501-7ECA-49F7-8778-74DA8B793EE3}">
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="G359" sqref="G359"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="G179" sqref="G179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4423,7 +4426,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>385</v>
       </c>
@@ -4439,13 +4442,16 @@
       <c r="F177" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G177" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E178" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>389</v>
       </c>
@@ -4461,13 +4467,16 @@
       <c r="F179" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G179" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E180" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>394</v>
       </c>
@@ -4484,12 +4493,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E182" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>398</v>
       </c>
@@ -4506,12 +4515,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E184" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>403</v>
       </c>
@@ -4528,12 +4537,12 @@
         <v>407</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E186" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>408</v>
       </c>
@@ -4550,12 +4559,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E188" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>412</v>
       </c>
@@ -4572,12 +4581,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E190" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>416</v>
       </c>
@@ -4594,7 +4603,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E192" t="s">
         <v>419</v>
       </c>

</xml_diff>

<commit_message>
Completed Binary Search Tree
</commit_message>
<xml_diff>
--- a/Exercise_Sequence.xlsx
+++ b/Exercise_Sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brind\Documents\HtDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB8E7D-E963-46A6-B64C-AA17CDC6EDE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2088E5E-E6F3-4B1E-A7E5-7B92CE971432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22016CAA-A539-451C-8737-08F3A468224D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="719">
   <si>
     <t>#</t>
   </si>
@@ -2188,6 +2188,9 @@
   </si>
   <si>
     <t>completed on 07-Nov</t>
+  </si>
+  <si>
+    <t>skipped</t>
   </si>
 </sst>
 </file>
@@ -2544,8 +2547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC50D501-7ECA-49F7-8778-74DA8B793EE3}">
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="G179" sqref="G179"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4492,6 +4495,9 @@
       <c r="F181" t="s">
         <v>253</v>
       </c>
+      <c r="G181" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E182" t="s">
@@ -4514,6 +4520,9 @@
       <c r="F183" t="s">
         <v>402</v>
       </c>
+      <c r="G183" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E184" t="s">
@@ -4536,6 +4545,9 @@
       <c r="F185" t="s">
         <v>407</v>
       </c>
+      <c r="G185" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E186" t="s">
@@ -4558,6 +4570,9 @@
       <c r="F187" t="s">
         <v>402</v>
       </c>
+      <c r="G187" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E188" t="s">
@@ -4580,6 +4595,9 @@
       <c r="F189" t="s">
         <v>402</v>
       </c>
+      <c r="G189" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E190" t="s">
@@ -4602,13 +4620,16 @@
       <c r="F191" t="s">
         <v>402</v>
       </c>
+      <c r="G191" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E192" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>420</v>
       </c>
@@ -4624,13 +4645,16 @@
       <c r="F193" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G193" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E194" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>424</v>
       </c>
@@ -4646,13 +4670,16 @@
       <c r="F195" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G195" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E196" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>428</v>
       </c>
@@ -4668,13 +4695,16 @@
       <c r="F197" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G197" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E198" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>432</v>
       </c>
@@ -4690,28 +4720,31 @@
       <c r="F199" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G199" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E200" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E201" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E202" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E203" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>439</v>
       </c>
@@ -4728,12 +4761,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E205" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>444</v>
       </c>
@@ -4750,12 +4783,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E207" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>448</v>
       </c>

</xml_diff>

<commit_message>
Completed arbitrary arity tree first example
</commit_message>
<xml_diff>
--- a/Exercise_Sequence.xlsx
+++ b/Exercise_Sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brind\Documents\HtDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC4B48-E463-4E8E-9D69-66710C00AABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00977978-5610-4A42-85BD-658E7A244D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22016CAA-A539-451C-8737-08F3A468224D}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="720">
   <si>
     <t>#</t>
   </si>
@@ -2192,6 +2191,9 @@
   </si>
   <si>
     <t>skipped</t>
+  </si>
+  <si>
+    <t>completed on 10-Nov</t>
   </si>
 </sst>
 </file>
@@ -2548,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC50D501-7ECA-49F7-8778-74DA8B793EE3}">
   <dimension ref="A1:G345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="G204" sqref="G204"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="E200" sqref="E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4761,6 +4763,9 @@
       <c r="F204" t="s">
         <v>443</v>
       </c>
+      <c r="G204" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E205" t="s">

</xml_diff>